<commit_message>
Test Cases to Row 10 in Automation Excel Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginValuesMap.xlsx
+++ b/src/test/resources/testdata/LoginValuesMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testOpsJavaFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D3BB7B-096F-4522-8419-CB249951FB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D16651-C1B7-4B5D-B4BC-C11E5657C95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>AdminID</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>CSTest</t>
+  </si>
+  <si>
+    <t>CS TEST</t>
   </si>
 </sst>
 </file>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +466,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
End of Sean's contribution
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginValuesMap.xlsx
+++ b/src/test/resources/testdata/LoginValuesMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testOpsJavaFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D16651-C1B7-4B5D-B4BC-C11E5657C95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73B75F3-FBBA-4A35-96EE-080DCC6BD843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,12 +39,6 @@
     <t>LoginLabel</t>
   </si>
   <si>
-    <t>testSean</t>
-  </si>
-  <si>
-    <t>SEANTEST PROCTOR</t>
-  </si>
-  <si>
     <t>adminTest</t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>CS TEST</t>
+  </si>
+  <si>
+    <t>supplierTest</t>
+  </si>
+  <si>
+    <t>SUPPLIER TEST</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -440,44 +440,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>